<commit_message>
Incorporate new fuel economy standards, update vehicle buyer discount rate, and recalibrate TTS for passenger LDVs (issue #213)
</commit_message>
<xml_diff>
--- a/InputData/trans/VBDR/Veh Buyer Discount Rate.xlsx
+++ b/InputData/trans/VBDR/Veh Buyer Discount Rate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\VBDR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\VBDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D03AF9-A242-4BBC-BCFA-62936AEA3897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="21075" windowHeight="13110"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,26 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>VBDR Vehicle Buyer Discount Rate</t>
   </si>
   <si>
-    <t>Source:</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Vehcile buyer discount rates vary tremendously by study.</t>
-  </si>
-  <si>
-    <t>The meta-analysis cited here includes studies that have found</t>
-  </si>
-  <si>
-    <t>discount rates as low as 0.2% and as high as 77% per year.</t>
-  </si>
-  <si>
     <t>The implied discount rate is sensitive to numerous assumptions</t>
   </si>
   <si>
@@ -55,12 +44,6 @@
     <t>might be.</t>
   </si>
   <si>
-    <t>We use a 7% discount rate, because this is the rate the</t>
-  </si>
-  <si>
-    <t>EPA chose to use (without endorsing this rate) for</t>
-  </si>
-  <si>
     <t>We use this rate for all vehicle types, since uncertainty</t>
   </si>
   <si>
@@ -73,21 +56,6 @@
     <t>a company that purchases trucks.</t>
   </si>
   <si>
-    <t>various calculations throughout their report.  (See p. 63.)</t>
-  </si>
-  <si>
-    <t>U.S. EPA</t>
-  </si>
-  <si>
-    <t>How Consumers Value Fuel Economy: A Literature Review</t>
-  </si>
-  <si>
-    <t>Page 63 (see Notes below)</t>
-  </si>
-  <si>
-    <t>https://nepis.epa.gov/Exe/ZyNET.exe/P1006V0O.txt?ZyActionD=ZyDocument&amp;Client=EPA&amp;Index=2006%20Thru%202010&amp;Docs=&amp;Query=&amp;Time=&amp;EndTime=&amp;SearchMethod=1&amp;TocRestrict=n&amp;Toc=&amp;TocEntry=&amp;QField=&amp;QFieldYear=&amp;QFieldMonth=&amp;QFieldDay=&amp;UseQField=&amp;IntQFieldOp=0&amp;ExtQFieldOp=0&amp;XmlQuery=&amp;File=D%3A%5CZYFILES%5CINDEX%20DATA%5C06THRU10%5CTXT%5C00000016%5CP1006V0O.txt&amp;User=ANONYMOUS&amp;Password=anonymous&amp;SortMethod=h%7C-&amp;MaximumDocuments=1&amp;FuzzyDegree=0&amp;ImageQuality=r75g8/r75g8/x150y150g16/i425&amp;Display=hpfr&amp;DefSeekPage=x&amp;SearchBack=ZyActionL&amp;Back=ZyActionS&amp;BackDesc=Results%20page&amp;MaximumPages=1&amp;ZyEntry=2#</t>
-  </si>
-  <si>
     <t>LDVs</t>
   </si>
   <si>
@@ -107,12 +75,48 @@
   </si>
   <si>
     <t>Discount Rate (dimensionless)</t>
+  </si>
+  <si>
+    <t>Sources:</t>
+  </si>
+  <si>
+    <t>https://media.rff.org/documents/wp_21-27.pdf</t>
+  </si>
+  <si>
+    <t>Resources for the Future</t>
+  </si>
+  <si>
+    <t>How Much Do Consumers Value Fuel Cost Savings? Evidence from the Passenger Vehicle Leasing Market</t>
+  </si>
+  <si>
+    <t>page 23</t>
+  </si>
+  <si>
+    <t>Vehicle buyer discount rates vary tremendously by study.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use a value of 15%, as it falls between values of 12% and </t>
+  </si>
+  <si>
+    <t>greater than 17% in the studies cited above.</t>
+  </si>
+  <si>
+    <t>Leard et al.</t>
+  </si>
+  <si>
+    <t>How Much Do Consumers Value Fuel Economy and Performance? Evidence from Technology Adoption</t>
+  </si>
+  <si>
+    <t>PDF page 6</t>
+  </si>
+  <si>
+    <t>https://www.rff.org/publications/reports/how-much-do-consumers-value-fuel-economy-and-performance-evidence-from-technology-adoption/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -249,6 +253,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -284,6 +305,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -459,124 +497,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -586,72 +639,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>7.0000000000000007E-2</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>